<commit_message>
Ran linear multivariate regression
</commit_message>
<xml_diff>
--- a/SUB1 DSMCRIT overlap.xlsx
+++ b/SUB1 DSMCRIT overlap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mymac/PycharmProjects/TEDSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F35618-2306-9E4D-AEBD-DC6244D9585A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25206BD-26DF-9D4D-BB45-E408EDDF2D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9620" yWindow="500" windowWidth="19180" windowHeight="15880" xr2:uid="{D29971F3-94DB-6D43-A2F2-083A19EF39BF}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="22640" windowHeight="15880" xr2:uid="{D29971F3-94DB-6D43-A2F2-083A19EF39BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>SUB1=5</t>
   </si>
@@ -63,13 +63,31 @@
   </si>
   <si>
     <t>Unknown</t>
+  </si>
+  <si>
+    <t>Opioid Dep.</t>
+  </si>
+  <si>
+    <t>Opioid Abuse</t>
+  </si>
+  <si>
+    <t>All Others</t>
+  </si>
+  <si>
+    <t>Heroin</t>
+  </si>
+  <si>
+    <t>Non-script methadone</t>
+  </si>
+  <si>
+    <t>Other opioids</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -83,6 +101,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -92,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -100,13 +126,107 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,155 +541,188 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995C2CEA-0C4A-9741-96C2-B62DCE4DA259}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C3" s="4">
         <v>258691</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D3" s="5">
         <v>1477</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E3" s="5">
         <v>80705</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F3" s="5">
         <v>32645</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G3" s="5">
         <v>29746</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H3" s="6">
         <v>403264</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C4" s="7">
         <v>10048</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
         <v>4864</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F4" s="9">
         <v>3126</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G4" s="9">
         <v>2492</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H4" s="10">
         <v>20530</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C5" s="7">
         <v>63040</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9">
         <v>812099</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G5" s="9">
         <v>85109</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H5" s="10">
         <v>960248</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9">
         <v>22257</v>
       </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
         <v>458008</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H6" s="10">
         <v>480265</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C7" s="11">
         <v>331779</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D7" s="12">
         <v>1477</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E7" s="12">
         <v>107826</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F7" s="12">
         <v>847870</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G7" s="12">
         <v>575355</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H7" s="13">
         <v>1864307</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F7" s="1"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>